<commit_message>
edited videos, updated BOM, added Matlab plots
</commit_message>
<xml_diff>
--- a/hardware/SHVRIMPS_BOM.xlsx
+++ b/hardware/SHVRIMPS_BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/SHVRIMPS/SHVRIMPS/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5082FAC7-F5EC-DC43-8BD5-F93D379248D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C13159-7DD6-6C4B-B372-74217FE67CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAQ Module" sheetId="2" r:id="rId1"/>
     <sheet name="HV Board" sheetId="3" r:id="rId2"/>
-    <sheet name="Wires and Consumables" sheetId="4" r:id="rId3"/>
-    <sheet name="Enclosure and Mains Supply" sheetId="5" r:id="rId4"/>
+    <sheet name="Raspberry Pi + camera" sheetId="6" r:id="rId3"/>
+    <sheet name="Wires and Consumables" sheetId="4" r:id="rId4"/>
+    <sheet name="Enclosure and Mains Supply" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="202">
   <si>
     <t>Ref</t>
   </si>
@@ -415,9 +416,6 @@
     <t>L7809ABV</t>
   </si>
   <si>
-    <t>So</t>
-  </si>
-  <si>
     <t>https://uk.rs-online.com/web/p/solder-pastes/1466194</t>
   </si>
   <si>
@@ -614,16 +612,47 @@
   </si>
   <si>
     <t>Wire for internal wiring</t>
+  </si>
+  <si>
+    <t>https://www.raspberrypi.com/products/raspberry-pi-4-model-b/</t>
+  </si>
+  <si>
+    <t>https://thepihut.com/products/raspberry-pi-camera-module?src=raspberrypi</t>
+  </si>
+  <si>
+    <t>Total for 8 boards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4B</t>
+  </si>
+  <si>
+    <t>Pi Camera v2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other </t>
+  </si>
+  <si>
+    <t>PCB Stencil</t>
+  </si>
+  <si>
+    <t>Thin sheet of metal masking for solder paste application</t>
+  </si>
+  <si>
+    <t>Pi Screen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0_);[Red]\(&quot;£&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -767,25 +796,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,12 +980,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1133,13 +1144,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1495,16 +1505,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
   </cols>
@@ -1529,7 +1541,7 @@
         <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H1" t="s">
         <v>73</v>
@@ -1551,16 +1563,16 @@
       <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F2" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>25.86</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <f t="shared" ref="I2:I26" si="0">H2*B2</f>
         <v>25.86</v>
       </c>
@@ -1579,18 +1591,18 @@
         <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H3" s="3">
+        <v>160</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.34399999999999997</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <f t="shared" si="0"/>
         <v>4.4719999999999995</v>
       </c>
@@ -1609,18 +1621,18 @@
         <v>76</v>
       </c>
       <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
         <v>176</v>
       </c>
-      <c r="F4" t="s">
-        <v>177</v>
-      </c>
       <c r="G4" t="s">
-        <v>161</v>
-      </c>
-      <c r="H4" s="3">
+        <v>160</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.17599999999999999</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <f t="shared" si="0"/>
         <v>0.87999999999999989</v>
       </c>
@@ -1639,15 +1651,15 @@
         <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H5" s="3">
+        <v>160</v>
+      </c>
+      <c r="H5" s="2">
         <v>0.24399999999999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
         <v>0.48799999999999999</v>
       </c>
@@ -1662,19 +1674,20 @@
       <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="E6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="2">
         <v>0.109</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <f t="shared" si="0"/>
         <v>0.109</v>
       </c>
@@ -1689,19 +1702,20 @@
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E7" t="s">
-        <v>180</v>
-      </c>
-      <c r="G7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H7" s="5">
+      <c r="E7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="2">
         <v>0.185</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
         <v>0.185</v>
       </c>
@@ -1716,22 +1730,22 @@
       <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>0.254</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <f>H8*B8</f>
         <v>0.254</v>
       </c>
@@ -1746,22 +1760,22 @@
       <c r="C9" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="F9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H9" s="2">
         <v>1.45</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <f t="shared" si="0"/>
         <v>1.45</v>
       </c>
@@ -1773,22 +1787,22 @@
       <c r="C10" t="s">
         <v>93</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F10" t="s">
-        <v>146</v>
-      </c>
-      <c r="G10" t="s">
-        <v>163</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="F10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" s="2">
         <v>0.53800000000000003</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <f t="shared" si="0"/>
         <v>0.53800000000000003</v>
       </c>
@@ -1803,22 +1817,22 @@
       <c r="C11" t="s">
         <v>94</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F11" t="s">
-        <v>147</v>
-      </c>
-      <c r="G11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="F11" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="2">
         <v>4.29</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <f t="shared" si="0"/>
         <v>12.870000000000001</v>
       </c>
@@ -1830,19 +1844,20 @@
       <c r="C12" t="s">
         <v>95</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G12" t="s">
-        <v>163</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="F12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H12" s="2">
         <v>1.24</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <f t="shared" si="0"/>
         <v>3.7199999999999998</v>
       </c>
@@ -1857,22 +1872,22 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F13" t="s">
-        <v>141</v>
-      </c>
-      <c r="G13" t="s">
-        <v>163</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="F13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="2">
         <v>1.1399999999999999</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <f t="shared" si="0"/>
         <v>1.1399999999999999</v>
       </c>
@@ -1884,19 +1899,20 @@
       <c r="C14" t="s">
         <v>96</v>
       </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G14" t="s">
-        <v>163</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="F14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" s="2">
         <v>0.38600000000000001</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <f t="shared" si="0"/>
         <v>0.38600000000000001</v>
       </c>
@@ -1909,24 +1925,24 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E15" t="s">
-        <v>169</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G15" t="s">
-        <v>161</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="F15" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H15" s="2">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <f t="shared" si="0"/>
         <v>0.252</v>
       </c>
@@ -1939,29 +1955,29 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
-      </c>
-      <c r="D16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>82</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F16" t="s">
-        <v>164</v>
-      </c>
-      <c r="G16" t="s">
-        <v>161</v>
-      </c>
-      <c r="H16" s="3">
+        <v>148</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" s="2">
         <v>0.253</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <f t="shared" si="0"/>
         <v>0.253</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1969,26 +1985,27 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E17" t="s">
-        <v>167</v>
-      </c>
-      <c r="G17" t="s">
-        <v>161</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="E17" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="2">
         <v>0.20200000000000001</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <f t="shared" si="0"/>
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1998,19 +2015,21 @@
       <c r="C18" t="s">
         <v>55</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E18" t="s">
-        <v>170</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3">
+      <c r="E18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -2020,24 +2039,25 @@
       <c r="C19" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>86</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F19" t="s">
-        <v>155</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <f t="shared" si="0"/>
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -2047,25 +2067,27 @@
       <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G20" t="s">
-        <v>165</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F20" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -2075,25 +2097,27 @@
       <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F21" t="s">
-        <v>151</v>
-      </c>
-      <c r="G21" t="s">
-        <v>165</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2103,28 +2127,28 @@
       <c r="C22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F22" t="s">
-        <v>152</v>
-      </c>
-      <c r="G22" t="s">
-        <v>165</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="F22" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="2">
         <f>1.03*1.25</f>
         <v>1.2875000000000001</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <f t="shared" si="0"/>
         <v>1.2875000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -2134,27 +2158,27 @@
       <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F23" t="s">
-        <v>153</v>
-      </c>
-      <c r="G23" t="s">
-        <v>158</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="F23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="2">
         <v>4.38</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <f t="shared" si="0"/>
         <v>8.76</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -2174,17 +2198,17 @@
         <v>68</v>
       </c>
       <c r="G24" t="s">
-        <v>159</v>
-      </c>
-      <c r="H24" s="3">
+        <v>158</v>
+      </c>
+      <c r="H24" s="2">
         <v>21.65</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <f t="shared" si="0"/>
         <v>21.65</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2204,76 +2228,171 @@
         <v>70</v>
       </c>
       <c r="G25" t="s">
-        <v>166</v>
-      </c>
-      <c r="H25" s="3">
+        <v>165</v>
+      </c>
+      <c r="H25" s="2">
         <v>1.17</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" t="s">
         <v>129</v>
       </c>
-      <c r="D26" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" t="s">
-        <v>130</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <f>6.54/5</f>
         <v>1.3080000000000001</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="2">
         <f t="shared" si="0"/>
         <v>1.3080000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H27" t="s">
-        <v>162</v>
-      </c>
-      <c r="I27" s="3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+      <c r="H27" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>161</v>
+      </c>
+      <c r="I28" s="2">
         <f>SUM(I2:I26)</f>
-        <v>88.157499999999999</v>
-      </c>
+        <v>89.183500000000009</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E30" s="1"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D33" s="2"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D34" s="2"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E36" s="1"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E37" s="1"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="I40" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="20" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1"/>
-    <hyperlink ref="E11" r:id="rId2"/>
-    <hyperlink ref="E13" r:id="rId3"/>
-    <hyperlink ref="E24" r:id="rId4"/>
-    <hyperlink ref="E23" r:id="rId5"/>
-    <hyperlink ref="E22" r:id="rId6"/>
-    <hyperlink ref="E25" r:id="rId7"/>
-    <hyperlink ref="E8" r:id="rId8"/>
-    <hyperlink ref="E20" r:id="rId9"/>
-    <hyperlink ref="E2" r:id="rId10"/>
-    <hyperlink ref="E9" r:id="rId11"/>
-    <hyperlink ref="E10" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E16" r:id="rId14"/>
-    <hyperlink ref="E19" r:id="rId15"/>
+    <hyperlink ref="E12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E24" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E25" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E2" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E21" r:id="rId16" xr:uid="{897280EB-A452-6347-9F4F-6AE5E966771A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2309,7 +2428,7 @@
         <v>108</v>
       </c>
       <c r="G2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H2" t="s">
         <v>73</v>
@@ -2332,7 +2451,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H3">
         <v>0.193</v>
@@ -2356,7 +2475,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H4">
         <v>0.31900000000000001</v>
@@ -2380,7 +2499,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H5">
         <v>0.46200000000000002</v>
@@ -2398,16 +2517,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
         <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6">
         <v>0.75600000000000001</v>
@@ -2419,22 +2538,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
         <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H7">
         <v>1.81</v>
@@ -2461,7 +2580,7 @@
         <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H8">
         <v>1.1399999999999999</v>
@@ -2473,7 +2592,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2488,7 +2607,7 @@
         <v>101</v>
       </c>
       <c r="F9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9">
         <v>0.38600000000000001</v>
@@ -2515,7 +2634,7 @@
         <v>111</v>
       </c>
       <c r="F10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H10">
         <v>2.5000000000000001E-2</v>
@@ -2542,7 +2661,7 @@
         <v>112</v>
       </c>
       <c r="F11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H11">
         <v>2.1000000000000001E-2</v>
@@ -2569,7 +2688,7 @@
         <v>110</v>
       </c>
       <c r="F12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H12">
         <v>8.4000000000000005E-2</v>
@@ -2617,7 +2736,7 @@
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H14">
         <v>0.66400000000000003</v>
@@ -2695,7 +2814,10 @@
         <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>180</v>
+      </c>
+      <c r="G17" t="s">
+        <v>198</v>
       </c>
       <c r="H17">
         <v>433.09</v>
@@ -2710,49 +2832,288 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" t="s">
         <v>129</v>
       </c>
-      <c r="D18" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" t="s">
-        <v>130</v>
+      <c r="H18">
+        <v>2</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I19">
         <f>SUM(I3:I18)</f>
-        <v>441.73499999999996</v>
+        <v>443.73499999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>194</v>
+      </c>
+      <c r="I20">
+        <f>I19*8</f>
+        <v>3549.8799999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1"/>
-    <hyperlink ref="E10" r:id="rId2"/>
-    <hyperlink ref="E11" r:id="rId3"/>
-    <hyperlink ref="E15" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
-    <hyperlink ref="E9" r:id="rId7"/>
-    <hyperlink ref="E6" r:id="rId8"/>
+    <hyperlink ref="E12" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E11" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E15" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833742FD-3AA8-714C-A69E-FB4A11087A29}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H2" s="3">
+        <v>65</v>
+      </c>
+      <c r="I2" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" s="3">
+        <v>26</v>
+      </c>
+      <c r="I3" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I8" s="3">
+        <f>SUM(I2:I7)</f>
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="2">
+        <v>40.25</v>
+      </c>
+      <c r="I2" s="2">
+        <f>H2</f>
+        <v>40.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="2">
+        <v>16.88</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I4" si="0">H3</f>
+        <v>16.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="2">
+        <v>18.62</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>18.62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6" s="3">
+        <f>SUM(I2:I5)</f>
+        <v>75.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2783,79 +3144,6 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="3">
-        <v>40.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="3">
-        <v>16.88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" t="s">
-        <v>188</v>
-      </c>
-      <c r="H4" s="3">
-        <v>18.62</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>126</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>